<commit_message>
Worked on Login Functionality
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Testcodeword1</t>
   </si>
@@ -36,6 +36,30 @@
   </si>
   <si>
     <t>Testcodeword4</t>
+  </si>
+  <si>
+    <t>Testcodeword5</t>
+  </si>
+  <si>
+    <t>Testcodeword6</t>
+  </si>
+  <si>
+    <t>Testcodeword7</t>
+  </si>
+  <si>
+    <t>Testcodeword8</t>
+  </si>
+  <si>
+    <t>Testcodeword9</t>
+  </si>
+  <si>
+    <t>Testcodeword10</t>
+  </si>
+  <si>
+    <t>Testcodeword11</t>
+  </si>
+  <si>
+    <t>Testcodeword12</t>
   </si>
 </sst>
 </file>
@@ -353,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,6 +408,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Displaying the dynamic student dashboard
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,71 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531373\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAF1106-882C-4A5F-B524-401AD8C72DB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD19AD9-0F01-4F5C-918B-957EA0001A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Testcodeword1</t>
-  </si>
-  <si>
-    <t>Testcodeword2</t>
-  </si>
-  <si>
-    <t>Testcodeword3</t>
-  </si>
-  <si>
-    <t>Testcodeword4</t>
-  </si>
-  <si>
-    <t>Testcodeword5</t>
-  </si>
-  <si>
-    <t>Testcodeword6</t>
-  </si>
-  <si>
-    <t>Testcodeword7</t>
-  </si>
-  <si>
-    <t>Testcodeword8</t>
-  </si>
-  <si>
-    <t>Testcodeword9</t>
-  </si>
-  <si>
-    <t>Testcodeword10</t>
-  </si>
-  <si>
-    <t>Testcodeword11</t>
-  </si>
-  <si>
-    <t>Testcodeword12</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,8 +102,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{E32EB8DE-4BA9-437E-B919-26DD904E2398}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -131,7 +160,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -143,7 +172,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -190,6 +219,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -225,6 +271,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,17 +439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EEFE03-D778-4EDA-9061-7E4542C8674C}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -438,16 +498,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made changes to the date variables so that the start and end date comup differently
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531373\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAF1106-882C-4A5F-B524-401AD8C72DB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F94D5B-69A6-477D-9A62-F49297E83D78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD19AD9-0F01-4F5C-918B-957EA0001A54}"/>
   </bookViews>
@@ -33,34 +33,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>DOG</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>ELEPHANT</t>
+  </si>
+  <si>
+    <t>FAN</t>
+  </si>
+  <si>
+    <t>GOAT</t>
+  </si>
+  <si>
+    <t>HILL</t>
+  </si>
+  <si>
+    <t>ICECREAM</t>
+  </si>
+  <si>
+    <t>JOKER</t>
   </si>
 </sst>
 </file>
@@ -443,29 +443,29 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on Adding codewords in existing codewordset
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,30 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531373\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\GDP-2\Seperate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F94D5B-69A6-477D-9A62-F49297E83D78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD19AD9-0F01-4F5C-918B-957EA0001A54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,40 +26,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>CAT</t>
-  </si>
-  <si>
-    <t>DOG</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>APPLE</t>
-  </si>
-  <si>
-    <t>ELEPHANT</t>
-  </si>
-  <si>
-    <t>FAN</t>
-  </si>
-  <si>
-    <t>GOAT</t>
-  </si>
-  <si>
-    <t>HILL</t>
-  </si>
-  <si>
-    <t>ICECREAM</t>
-  </si>
-  <si>
-    <t>JOKER</t>
+    <t>Testcodeword1</t>
+  </si>
+  <si>
+    <t>Testcodeword2</t>
+  </si>
+  <si>
+    <t>Testcodeword3</t>
+  </si>
+  <si>
+    <t>Testcodeword4</t>
+  </si>
+  <si>
+    <t>Testcodeword5</t>
+  </si>
+  <si>
+    <t>Testcodeword6</t>
+  </si>
+  <si>
+    <t>Testcodeword7</t>
+  </si>
+  <si>
+    <t>Testcodeword8</t>
+  </si>
+  <si>
+    <t>Testcodeword9</t>
+  </si>
+  <si>
+    <t>Testcodeword10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,36 +95,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{E32EB8DE-4BA9-437E-B919-26DD904E2398}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -160,7 +125,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -172,7 +137,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -219,23 +184,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -271,23 +219,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,33 +370,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EEFE03-D778-4EDA-9061-7E4542C8674C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A11:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Displaying the ack status
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,30 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531373\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\GDP-2\Seperate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F94D5B-69A6-477D-9A62-F49297E83D78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EDD19AD9-0F01-4F5C-918B-957EA0001A54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,40 +26,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>CAT</t>
-  </si>
-  <si>
-    <t>DOG</t>
-  </si>
-  <si>
-    <t>BAT</t>
-  </si>
-  <si>
-    <t>APPLE</t>
-  </si>
-  <si>
-    <t>ELEPHANT</t>
-  </si>
-  <si>
-    <t>FAN</t>
-  </si>
-  <si>
-    <t>GOAT</t>
-  </si>
-  <si>
-    <t>HILL</t>
-  </si>
-  <si>
-    <t>ICECREAM</t>
-  </si>
-  <si>
-    <t>JOKER</t>
+    <t>Testcodeword1</t>
+  </si>
+  <si>
+    <t>Testcodeword2</t>
+  </si>
+  <si>
+    <t>Testcodeword3</t>
+  </si>
+  <si>
+    <t>Testcodeword4</t>
+  </si>
+  <si>
+    <t>Testcodeword5</t>
+  </si>
+  <si>
+    <t>Testcodeword6</t>
+  </si>
+  <si>
+    <t>Testcodeword7</t>
+  </si>
+  <si>
+    <t>Testcodeword8</t>
+  </si>
+  <si>
+    <t>Testcodeword9</t>
+  </si>
+  <si>
+    <t>Testcodeword10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,36 +95,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{E32EB8DE-4BA9-437E-B919-26DD904E2398}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -160,7 +125,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -172,7 +137,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -219,23 +184,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -271,23 +219,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,33 +370,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EEFE03-D778-4EDA-9061-7E4542C8674C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A11:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Delete course n codewordset
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s530473\Desktop\GDP-2\Present\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhij\Documents\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52ABCF8-4C80-4654-AC39-58A9039D7933}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>APPLE</t>
   </si>
@@ -36,9 +37,6 @@
   </si>
   <si>
     <t>CHERRY</t>
-  </si>
-  <si>
-    <t>MANGO</t>
   </si>
   <si>
     <t>JACKFRUIT</t>
@@ -50,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -361,51 +359,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>